<commit_message>
Implementar carga de estudiantes desde CSV con validación
</commit_message>
<xml_diff>
--- a/Estudiantes.xlsx
+++ b/Estudiantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAFEYEF\Desktop\Taller1DevOps\TallerGit\Taller-Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C603D12-769B-43DA-8C65-3DFFCC5228C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9506BE38-D2D4-400D-B608-F9106665A1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,8 +52,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -81,10 +89,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -366,61 +375,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B7"/>
+  <dimension ref="A2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>4.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>3.8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>2.9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>4.2</v>
       </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>